<commit_message>
checking active sheet if that matters
</commit_message>
<xml_diff>
--- a/test4.xlsx
+++ b/test4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreitz\AppData\Local\Programs\Python\Python36-32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreitz\AppData\Local\Programs\Python\Python36-32\Student-Data-Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="38" r:id="rId1"/>
@@ -8676,7 +8676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E427"/>
   <sheetViews>
-    <sheetView topLeftCell="A422" workbookViewId="0">
+    <sheetView topLeftCell="A426" workbookViewId="0">
       <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
@@ -21380,7 +21380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -23112,8 +23112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24484,8 +24484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
"Yay! Completion Agency Search works"
</commit_message>
<xml_diff>
--- a/test4.xlsx
+++ b/test4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="38" r:id="rId1"/>
@@ -8676,8 +8676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E427"/>
   <sheetViews>
-    <sheetView topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15968,7 +15968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -23112,8 +23112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>